<commit_message>
AutoCommit_26 марта 2024 г. 12:30:36_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-422_ТерВер.xlsx
+++ b/_2ИСИП-422_ТерВер.xlsx
@@ -498,10 +498,10 @@
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2:G2"/>
+      <selection pane="bottomRight" activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -815,9 +815,15 @@
       <c r="B23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
+      <c r="C23" s="2">
+        <v>5</v>
+      </c>
+      <c r="D23" s="2">
+        <v>5</v>
+      </c>
+      <c r="E23" s="2">
+        <v>5</v>
+      </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_29 марта 2024 г. 12:22:49_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-422_ТерВер.xlsx
+++ b/_2ИСИП-422_ТерВер.xlsx
@@ -498,10 +498,10 @@
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F23" sqref="F23"/>
+      <selection pane="bottomRight" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -605,9 +605,15 @@
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+      <c r="C8" s="2">
+        <v>5</v>
+      </c>
+      <c r="D8" s="2">
+        <v>5</v>
+      </c>
+      <c r="E8" s="2">
+        <v>5</v>
+      </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
@@ -773,10 +779,18 @@
       <c r="B20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
+      <c r="C20" s="2">
+        <v>5</v>
+      </c>
+      <c r="D20" s="2">
+        <v>5</v>
+      </c>
+      <c r="E20" s="2">
+        <v>5</v>
+      </c>
+      <c r="F20" s="2">
+        <v>5</v>
+      </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
@@ -919,10 +933,18 @@
       <c r="B30" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
+      <c r="C30" s="2">
+        <v>5</v>
+      </c>
+      <c r="D30" s="2">
+        <v>5</v>
+      </c>
+      <c r="E30" s="2">
+        <v>5</v>
+      </c>
+      <c r="F30" s="2">
+        <v>5</v>
+      </c>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>

</xml_diff>

<commit_message>
AutoCommit_29 марта 2024 г. 12:25:18_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-422_ТерВер.xlsx
+++ b/_2ИСИП-422_ТерВер.xlsx
@@ -498,10 +498,10 @@
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F21" sqref="F21"/>
+      <selection pane="bottomRight" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -577,9 +577,15 @@
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+      <c r="C6" s="2">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2">
+        <v>5</v>
+      </c>
+      <c r="E6" s="2">
+        <v>5</v>
+      </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
@@ -667,10 +673,18 @@
       <c r="B12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+      <c r="C12" s="2">
+        <v>5</v>
+      </c>
+      <c r="D12" s="2">
+        <v>5</v>
+      </c>
+      <c r="E12" s="2">
+        <v>5</v>
+      </c>
+      <c r="F12" s="2">
+        <v>5</v>
+      </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
@@ -709,10 +723,18 @@
       <c r="B15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
+      <c r="C15" s="2">
+        <v>5</v>
+      </c>
+      <c r="D15" s="2">
+        <v>5</v>
+      </c>
+      <c r="E15" s="2">
+        <v>5</v>
+      </c>
+      <c r="F15" s="2">
+        <v>5</v>
+      </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
@@ -751,10 +773,18 @@
       <c r="B18" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
+      <c r="C18" s="2">
+        <v>5</v>
+      </c>
+      <c r="D18" s="2">
+        <v>5</v>
+      </c>
+      <c r="E18" s="2">
+        <v>5</v>
+      </c>
+      <c r="F18" s="2">
+        <v>5</v>
+      </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
@@ -849,10 +879,18 @@
       <c r="B24" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
+      <c r="C24" s="2">
+        <v>5</v>
+      </c>
+      <c r="D24" s="2">
+        <v>5</v>
+      </c>
+      <c r="E24" s="2">
+        <v>5</v>
+      </c>
+      <c r="F24" s="2">
+        <v>5</v>
+      </c>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>

</xml_diff>

<commit_message>
AutoCommit_29 марта 2024 г. 13:33:22_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-422_ТерВер.xlsx
+++ b/_2ИСИП-422_ТерВер.xlsx
@@ -501,7 +501,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F6" sqref="F6"/>
+      <selection pane="bottomRight" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -563,10 +563,18 @@
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+      <c r="C5" s="2">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2">
+        <v>5</v>
+      </c>
+      <c r="E5" s="2">
+        <v>5</v>
+      </c>
+      <c r="F5" s="2">
+        <v>5</v>
+      </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
@@ -695,11 +703,21 @@
       <c r="B13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
+      <c r="C13" s="2">
+        <v>5</v>
+      </c>
+      <c r="D13" s="2">
+        <v>5</v>
+      </c>
+      <c r="E13" s="2">
+        <v>5</v>
+      </c>
+      <c r="F13" s="2">
+        <v>5</v>
+      </c>
+      <c r="G13" s="2">
+        <v>5</v>
+      </c>
       <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:8" ht="13" x14ac:dyDescent="0.25">
@@ -745,11 +763,21 @@
       <c r="B16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
+      <c r="C16" s="2">
+        <v>5</v>
+      </c>
+      <c r="D16" s="2">
+        <v>5</v>
+      </c>
+      <c r="E16" s="2">
+        <v>5</v>
+      </c>
+      <c r="F16" s="2">
+        <v>5</v>
+      </c>
+      <c r="G16" s="2">
+        <v>5</v>
+      </c>
       <c r="H16" s="2"/>
     </row>
     <row r="17" spans="1:8" ht="13" x14ac:dyDescent="0.25">
@@ -759,11 +787,21 @@
       <c r="B17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
+      <c r="C17" s="2">
+        <v>5</v>
+      </c>
+      <c r="D17" s="2">
+        <v>5</v>
+      </c>
+      <c r="E17" s="2">
+        <v>5</v>
+      </c>
+      <c r="F17" s="2">
+        <v>5</v>
+      </c>
+      <c r="G17" s="2">
+        <v>5</v>
+      </c>
       <c r="H17" s="2"/>
     </row>
     <row r="18" spans="1:8" ht="13" x14ac:dyDescent="0.25">
@@ -915,9 +953,15 @@
       <c r="B26" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
+      <c r="C26" s="2">
+        <v>5</v>
+      </c>
+      <c r="D26" s="2">
+        <v>5</v>
+      </c>
+      <c r="E26" s="2">
+        <v>5</v>
+      </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
@@ -957,11 +1001,21 @@
       <c r="B29" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
+      <c r="C29" s="2">
+        <v>5</v>
+      </c>
+      <c r="D29" s="2">
+        <v>5</v>
+      </c>
+      <c r="E29" s="2">
+        <v>5</v>
+      </c>
+      <c r="F29" s="2">
+        <v>5</v>
+      </c>
+      <c r="G29" s="2">
+        <v>5</v>
+      </c>
       <c r="H29" s="2"/>
     </row>
     <row r="30" spans="1:8" ht="13" x14ac:dyDescent="0.25">
@@ -993,11 +1047,21 @@
       <c r="B31" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
+      <c r="C31" s="2">
+        <v>5</v>
+      </c>
+      <c r="D31" s="2">
+        <v>5</v>
+      </c>
+      <c r="E31" s="2">
+        <v>5</v>
+      </c>
+      <c r="F31" s="2">
+        <v>5</v>
+      </c>
+      <c r="G31" s="2">
+        <v>5</v>
+      </c>
       <c r="H31" s="2"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
AutoCommit_29 марта 2024 г. 13:44:33_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-422_ТерВер.xlsx
+++ b/_2ИСИП-422_ТерВер.xlsx
@@ -501,7 +501,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H5" sqref="H5"/>
+      <selection pane="bottomRight" activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -653,10 +653,18 @@
       <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+      <c r="C10" s="2">
+        <v>5</v>
+      </c>
+      <c r="D10" s="2">
+        <v>5</v>
+      </c>
+      <c r="E10" s="2">
+        <v>5</v>
+      </c>
+      <c r="F10" s="2">
+        <v>5</v>
+      </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
@@ -906,8 +914,12 @@
       <c r="E23" s="2">
         <v>5</v>
       </c>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
+      <c r="F23" s="2">
+        <v>5</v>
+      </c>
+      <c r="G23" s="2">
+        <v>5</v>
+      </c>
       <c r="H23" s="2"/>
     </row>
     <row r="24" spans="1:8" ht="13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
AutoCommit_3 апреля 2024 г. 10:16:15_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-422_ТерВер.xlsx
+++ b/_2ИСИП-422_ТерВер.xlsx
@@ -501,7 +501,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H23" sqref="H23"/>
+      <selection pane="bottomRight" activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -639,11 +639,21 @@
       <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
+      <c r="C9" s="2">
+        <v>5</v>
+      </c>
+      <c r="D9" s="2">
+        <v>5</v>
+      </c>
+      <c r="E9" s="2">
+        <v>5</v>
+      </c>
+      <c r="F9" s="2">
+        <v>5</v>
+      </c>
+      <c r="G9" s="2">
+        <v>5</v>
+      </c>
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" ht="13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
AutoCommit_5 апреля 2024 г. 13:49:48_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-422_ТерВер.xlsx
+++ b/_2ИСИП-422_ТерВер.xlsx
@@ -501,7 +501,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G22" sqref="G22"/>
+      <selection pane="bottomRight" activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -963,10 +963,16 @@
       <c r="B25" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="2"/>
+      <c r="C25" s="2">
+        <v>5</v>
+      </c>
       <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
+      <c r="E25" s="2">
+        <v>5</v>
+      </c>
+      <c r="F25" s="2">
+        <v>5</v>
+      </c>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>

</xml_diff>

<commit_message>
AutoCommit_11 апреля 2024 г. 17:11:20_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-422_ТерВер.xlsx
+++ b/_2ИСИП-422_ТерВер.xlsx
@@ -151,12 +151,18 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -195,7 +201,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -207,6 +213,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -513,13 +522,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="K4" sqref="K4"/>
+      <selection pane="bottomRight" activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -529,12 +538,12 @@
     <col min="3" max="8" width="5.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="29" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
         <v>29</v>
       </c>
@@ -558,7 +567,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -566,17 +575,25 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="C4" s="5">
+        <v>0</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0</v>
+      </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="J4">
@@ -586,24 +603,27 @@
       <c r="K4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="2">
-        <v>5</v>
-      </c>
-      <c r="D5" s="2">
-        <v>5</v>
-      </c>
-      <c r="E5" s="2">
-        <v>5</v>
-      </c>
-      <c r="F5" s="2">
+      <c r="C5" s="5">
+        <v>5</v>
+      </c>
+      <c r="D5" s="5">
+        <v>5</v>
+      </c>
+      <c r="E5" s="5">
+        <v>5</v>
+      </c>
+      <c r="F5" s="5">
         <v>5</v>
       </c>
       <c r="G5" s="2"/>
@@ -615,24 +635,29 @@
       <c r="K5">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="2">
-        <v>5</v>
-      </c>
-      <c r="D6" s="2">
-        <v>5</v>
-      </c>
-      <c r="E6" s="2">
-        <v>5</v>
-      </c>
-      <c r="F6" s="2"/>
+      <c r="C6" s="5">
+        <v>5</v>
+      </c>
+      <c r="D6" s="5">
+        <v>5</v>
+      </c>
+      <c r="E6" s="5">
+        <v>5</v>
+      </c>
+      <c r="F6" s="5">
+        <v>0</v>
+      </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="J6">
@@ -642,18 +667,29 @@
       <c r="K6">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+      <c r="C7" s="5">
+        <v>0</v>
+      </c>
+      <c r="D7" s="5">
+        <v>0</v>
+      </c>
+      <c r="E7" s="5">
+        <v>0</v>
+      </c>
+      <c r="F7" s="5">
+        <v>0</v>
+      </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="J7">
@@ -663,24 +699,29 @@
       <c r="K7">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="2">
-        <v>5</v>
-      </c>
-      <c r="D8" s="2">
-        <v>5</v>
-      </c>
-      <c r="E8" s="2">
-        <v>5</v>
-      </c>
-      <c r="F8" s="2"/>
+      <c r="C8" s="5">
+        <v>5</v>
+      </c>
+      <c r="D8" s="5">
+        <v>5</v>
+      </c>
+      <c r="E8" s="5">
+        <v>5</v>
+      </c>
+      <c r="F8" s="5">
+        <v>0</v>
+      </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="J8">
@@ -690,24 +731,27 @@
       <c r="K8">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="2">
-        <v>5</v>
-      </c>
-      <c r="D9" s="2">
-        <v>5</v>
-      </c>
-      <c r="E9" s="2">
-        <v>5</v>
-      </c>
-      <c r="F9" s="2">
+      <c r="C9" s="5">
+        <v>5</v>
+      </c>
+      <c r="D9" s="5">
+        <v>5</v>
+      </c>
+      <c r="E9" s="5">
+        <v>5</v>
+      </c>
+      <c r="F9" s="5">
         <v>5</v>
       </c>
       <c r="G9" s="2">
@@ -721,24 +765,27 @@
       <c r="K9">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="2">
-        <v>5</v>
-      </c>
-      <c r="D10" s="2">
-        <v>5</v>
-      </c>
-      <c r="E10" s="2">
-        <v>5</v>
-      </c>
-      <c r="F10" s="2">
+      <c r="C10" s="5">
+        <v>5</v>
+      </c>
+      <c r="D10" s="5">
+        <v>5</v>
+      </c>
+      <c r="E10" s="5">
+        <v>5</v>
+      </c>
+      <c r="F10" s="5">
         <v>5</v>
       </c>
       <c r="G10" s="2"/>
@@ -750,18 +797,29 @@
       <c r="K10">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+      <c r="C11" s="5">
+        <v>0</v>
+      </c>
+      <c r="D11" s="5">
+        <v>0</v>
+      </c>
+      <c r="E11" s="5">
+        <v>0</v>
+      </c>
+      <c r="F11" s="5">
+        <v>0</v>
+      </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="J11">
@@ -771,24 +829,27 @@
       <c r="K11">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="2">
-        <v>5</v>
-      </c>
-      <c r="D12" s="2">
-        <v>5</v>
-      </c>
-      <c r="E12" s="2">
-        <v>5</v>
-      </c>
-      <c r="F12" s="2">
+      <c r="C12" s="5">
+        <v>5</v>
+      </c>
+      <c r="D12" s="5">
+        <v>5</v>
+      </c>
+      <c r="E12" s="5">
+        <v>5</v>
+      </c>
+      <c r="F12" s="5">
         <v>5</v>
       </c>
       <c r="G12" s="2"/>
@@ -800,24 +861,27 @@
       <c r="K12">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="2">
-        <v>5</v>
-      </c>
-      <c r="D13" s="2">
-        <v>5</v>
-      </c>
-      <c r="E13" s="2">
-        <v>5</v>
-      </c>
-      <c r="F13" s="2">
+      <c r="C13" s="5">
+        <v>5</v>
+      </c>
+      <c r="D13" s="5">
+        <v>5</v>
+      </c>
+      <c r="E13" s="5">
+        <v>5</v>
+      </c>
+      <c r="F13" s="5">
         <v>5</v>
       </c>
       <c r="G13" s="2">
@@ -831,18 +895,29 @@
       <c r="K13">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>11</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+      <c r="C14" s="5">
+        <v>0</v>
+      </c>
+      <c r="D14" s="5">
+        <v>0</v>
+      </c>
+      <c r="E14" s="5">
+        <v>0</v>
+      </c>
+      <c r="F14" s="5">
+        <v>0</v>
+      </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="J14">
@@ -852,24 +927,27 @@
       <c r="K14">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>12</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="2">
-        <v>5</v>
-      </c>
-      <c r="D15" s="2">
-        <v>5</v>
-      </c>
-      <c r="E15" s="2">
-        <v>5</v>
-      </c>
-      <c r="F15" s="2">
+      <c r="C15" s="5">
+        <v>5</v>
+      </c>
+      <c r="D15" s="5">
+        <v>5</v>
+      </c>
+      <c r="E15" s="5">
+        <v>5</v>
+      </c>
+      <c r="F15" s="5">
         <v>5</v>
       </c>
       <c r="G15" s="2"/>
@@ -881,24 +959,27 @@
       <c r="K15">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>13</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="2">
-        <v>5</v>
-      </c>
-      <c r="D16" s="2">
-        <v>5</v>
-      </c>
-      <c r="E16" s="2">
-        <v>5</v>
-      </c>
-      <c r="F16" s="2">
+      <c r="C16" s="5">
+        <v>5</v>
+      </c>
+      <c r="D16" s="5">
+        <v>5</v>
+      </c>
+      <c r="E16" s="5">
+        <v>5</v>
+      </c>
+      <c r="F16" s="5">
         <v>5</v>
       </c>
       <c r="G16" s="2">
@@ -912,24 +993,27 @@
       <c r="K16">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>14</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="2">
-        <v>5</v>
-      </c>
-      <c r="D17" s="2">
-        <v>5</v>
-      </c>
-      <c r="E17" s="2">
-        <v>5</v>
-      </c>
-      <c r="F17" s="2">
+      <c r="C17" s="5">
+        <v>5</v>
+      </c>
+      <c r="D17" s="5">
+        <v>5</v>
+      </c>
+      <c r="E17" s="5">
+        <v>5</v>
+      </c>
+      <c r="F17" s="5">
         <v>5</v>
       </c>
       <c r="G17" s="2">
@@ -943,24 +1027,27 @@
       <c r="K17">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>15</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="2">
-        <v>5</v>
-      </c>
-      <c r="D18" s="2">
-        <v>5</v>
-      </c>
-      <c r="E18" s="2">
-        <v>5</v>
-      </c>
-      <c r="F18" s="2">
+      <c r="C18" s="5">
+        <v>5</v>
+      </c>
+      <c r="D18" s="5">
+        <v>5</v>
+      </c>
+      <c r="E18" s="5">
+        <v>5</v>
+      </c>
+      <c r="F18" s="5">
         <v>5</v>
       </c>
       <c r="G18" s="2"/>
@@ -972,18 +1059,29 @@
       <c r="K18">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>16</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
+      <c r="C19" s="5">
+        <v>0</v>
+      </c>
+      <c r="D19" s="5">
+        <v>0</v>
+      </c>
+      <c r="E19" s="5">
+        <v>0</v>
+      </c>
+      <c r="F19" s="5">
+        <v>0</v>
+      </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="J19">
@@ -993,24 +1091,27 @@
       <c r="K19">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>17</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="2">
-        <v>5</v>
-      </c>
-      <c r="D20" s="2">
-        <v>5</v>
-      </c>
-      <c r="E20" s="2">
-        <v>5</v>
-      </c>
-      <c r="F20" s="2">
+      <c r="C20" s="5">
+        <v>5</v>
+      </c>
+      <c r="D20" s="5">
+        <v>5</v>
+      </c>
+      <c r="E20" s="5">
+        <v>5</v>
+      </c>
+      <c r="F20" s="5">
         <v>5</v>
       </c>
       <c r="G20" s="2"/>
@@ -1022,18 +1123,29 @@
       <c r="K20">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>18</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
+      <c r="C21" s="5">
+        <v>0</v>
+      </c>
+      <c r="D21" s="5">
+        <v>0</v>
+      </c>
+      <c r="E21" s="5">
+        <v>0</v>
+      </c>
+      <c r="F21" s="5">
+        <v>0</v>
+      </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="J21">
@@ -1043,18 +1155,27 @@
       <c r="K21">
         <v>3</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>19</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2">
+      <c r="C22" s="5">
+        <v>0</v>
+      </c>
+      <c r="D22" s="5">
+        <v>0</v>
+      </c>
+      <c r="E22" s="5">
+        <v>0</v>
+      </c>
+      <c r="F22" s="5">
         <v>5</v>
       </c>
       <c r="G22" s="2"/>
@@ -1066,24 +1187,27 @@
       <c r="K22">
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>20</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="2">
-        <v>5</v>
-      </c>
-      <c r="D23" s="2">
-        <v>5</v>
-      </c>
-      <c r="E23" s="2">
-        <v>5</v>
-      </c>
-      <c r="F23" s="2">
+      <c r="C23" s="5">
+        <v>5</v>
+      </c>
+      <c r="D23" s="5">
+        <v>5</v>
+      </c>
+      <c r="E23" s="5">
+        <v>5</v>
+      </c>
+      <c r="F23" s="5">
         <v>5</v>
       </c>
       <c r="G23" s="2">
@@ -1097,24 +1221,27 @@
       <c r="K23">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>21</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="2">
-        <v>5</v>
-      </c>
-      <c r="D24" s="2">
-        <v>5</v>
-      </c>
-      <c r="E24" s="2">
-        <v>5</v>
-      </c>
-      <c r="F24" s="2">
+      <c r="C24" s="5">
+        <v>5</v>
+      </c>
+      <c r="D24" s="5">
+        <v>5</v>
+      </c>
+      <c r="E24" s="5">
+        <v>5</v>
+      </c>
+      <c r="F24" s="5">
         <v>5</v>
       </c>
       <c r="G24" s="2"/>
@@ -1126,22 +1253,27 @@
       <c r="K24">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>22</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="2">
-        <v>5</v>
-      </c>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2">
-        <v>5</v>
-      </c>
-      <c r="F25" s="2">
+      <c r="C25" s="5">
+        <v>5</v>
+      </c>
+      <c r="D25" s="5">
+        <v>0</v>
+      </c>
+      <c r="E25" s="5">
+        <v>5</v>
+      </c>
+      <c r="F25" s="5">
         <v>5</v>
       </c>
       <c r="G25" s="2"/>
@@ -1153,24 +1285,29 @@
       <c r="K25">
         <v>4</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>23</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="2">
-        <v>5</v>
-      </c>
-      <c r="D26" s="2">
-        <v>5</v>
-      </c>
-      <c r="E26" s="2">
-        <v>5</v>
-      </c>
-      <c r="F26" s="2"/>
+      <c r="C26" s="5">
+        <v>5</v>
+      </c>
+      <c r="D26" s="5">
+        <v>5</v>
+      </c>
+      <c r="E26" s="5">
+        <v>5</v>
+      </c>
+      <c r="F26" s="5">
+        <v>0</v>
+      </c>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="J26">
@@ -1180,18 +1317,29 @@
       <c r="K26">
         <v>4</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>24</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
+      <c r="C27" s="5">
+        <v>0</v>
+      </c>
+      <c r="D27" s="5">
+        <v>0</v>
+      </c>
+      <c r="E27" s="5">
+        <v>0</v>
+      </c>
+      <c r="F27" s="5">
+        <v>0</v>
+      </c>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
       <c r="J27">
@@ -1201,18 +1349,29 @@
       <c r="K27">
         <v>3</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>25</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
+      <c r="C28" s="5">
+        <v>0</v>
+      </c>
+      <c r="D28" s="5">
+        <v>0</v>
+      </c>
+      <c r="E28" s="5">
+        <v>0</v>
+      </c>
+      <c r="F28" s="5">
+        <v>0</v>
+      </c>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="J28">
@@ -1222,24 +1381,27 @@
       <c r="K28">
         <v>3</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>26</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C29" s="2">
-        <v>5</v>
-      </c>
-      <c r="D29" s="2">
-        <v>5</v>
-      </c>
-      <c r="E29" s="2">
-        <v>5</v>
-      </c>
-      <c r="F29" s="2">
+      <c r="C29" s="5">
+        <v>5</v>
+      </c>
+      <c r="D29" s="5">
+        <v>5</v>
+      </c>
+      <c r="E29" s="5">
+        <v>5</v>
+      </c>
+      <c r="F29" s="5">
         <v>5</v>
       </c>
       <c r="G29" s="2">
@@ -1253,24 +1415,27 @@
       <c r="K29">
         <v>5</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>27</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C30" s="2">
-        <v>5</v>
-      </c>
-      <c r="D30" s="2">
-        <v>5</v>
-      </c>
-      <c r="E30" s="2">
-        <v>5</v>
-      </c>
-      <c r="F30" s="2">
+      <c r="C30" s="5">
+        <v>5</v>
+      </c>
+      <c r="D30" s="5">
+        <v>5</v>
+      </c>
+      <c r="E30" s="5">
+        <v>5</v>
+      </c>
+      <c r="F30" s="5">
         <v>5</v>
       </c>
       <c r="G30" s="2"/>
@@ -1282,24 +1447,27 @@
       <c r="K30">
         <v>5</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>28</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C31" s="2">
-        <v>5</v>
-      </c>
-      <c r="D31" s="2">
-        <v>5</v>
-      </c>
-      <c r="E31" s="2">
-        <v>5</v>
-      </c>
-      <c r="F31" s="2">
+      <c r="C31" s="5">
+        <v>5</v>
+      </c>
+      <c r="D31" s="5">
+        <v>5</v>
+      </c>
+      <c r="E31" s="5">
+        <v>5</v>
+      </c>
+      <c r="F31" s="5">
         <v>5</v>
       </c>
       <c r="G31" s="2">
@@ -1313,8 +1481,11 @@
       <c r="K31">
         <v>5</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>

</xml_diff>

<commit_message>
AutoCommit_12 апреля 2024 г. 12:46:44_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-422_ТерВер.xlsx
+++ b/_2ИСИП-422_ТерВер.xlsx
@@ -525,10 +525,10 @@
   <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="L32" sqref="L32"/>
+      <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1305,14 +1305,16 @@
       <c r="E26" s="5">
         <v>5</v>
       </c>
-      <c r="F26" s="5">
-        <v>0</v>
-      </c>
-      <c r="G26" s="2"/>
+      <c r="F26" s="2">
+        <v>5</v>
+      </c>
+      <c r="G26" s="2">
+        <v>5</v>
+      </c>
       <c r="H26" s="2"/>
       <c r="J26">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="K26">
         <v>4</v>

</xml_diff>

<commit_message>
AutoCommit_16 апреля 2024 г. 12:21:19_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-422_ТерВер.xlsx
+++ b/_2ИСИП-422_ТерВер.xlsx
@@ -78,9 +78,6 @@
     <t>Рустан Вячеслав</t>
   </si>
   <si>
-    <t>Саитов Артур</t>
-  </si>
-  <si>
     <t>Сидаков Али</t>
   </si>
   <si>
@@ -127,6 +124,9 @@
   </si>
   <si>
     <t>тк</t>
+  </si>
+  <si>
+    <t>Саитов Артур (Филипов...)</t>
   </si>
 </sst>
 </file>
@@ -525,10 +525,10 @@
   <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomRight" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -545,26 +545,26 @@
     </row>
     <row r="2" spans="1:12" ht="29" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="H2" s="1"/>
       <c r="J2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="13" x14ac:dyDescent="0.25">
@@ -1164,7 +1164,7 @@
         <v>19</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="C22" s="5">
         <v>0</v>
@@ -1196,7 +1196,7 @@
         <v>20</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C23" s="5">
         <v>5</v>
@@ -1230,7 +1230,7 @@
         <v>21</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C24" s="5">
         <v>5</v>
@@ -1262,7 +1262,7 @@
         <v>22</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C25" s="5">
         <v>5</v>
@@ -1294,7 +1294,7 @@
         <v>23</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C26" s="5">
         <v>5</v>
@@ -1328,7 +1328,7 @@
         <v>24</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C27" s="5">
         <v>0</v>
@@ -1360,20 +1360,12 @@
         <v>25</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C28" s="5">
-        <v>0</v>
-      </c>
-      <c r="D28" s="5">
-        <v>0</v>
-      </c>
-      <c r="E28" s="5">
-        <v>0</v>
-      </c>
-      <c r="F28" s="5">
-        <v>0</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="J28">
@@ -1392,7 +1384,7 @@
         <v>26</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C29" s="5">
         <v>5</v>
@@ -1426,7 +1418,7 @@
         <v>27</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C30" s="5">
         <v>5</v>
@@ -1458,7 +1450,7 @@
         <v>28</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C31" s="5">
         <v>5</v>

</xml_diff>

<commit_message>
AutoCommit_14 июня 2024 г. 9:02:09_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-422_ТерВер.xlsx
+++ b/_2ИСИП-422_ТерВер.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>2ИСИП-422: Теория вероятностей и математическая статистика (Сибирев И. В.) - II семестр</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t>лаб1</t>
+  </si>
+  <si>
+    <t>Хочу 4</t>
   </si>
 </sst>
 </file>
@@ -539,10 +542,10 @@
   <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J6" sqref="J6"/>
+      <selection pane="bottomRight" activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -599,20 +602,25 @@
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="5">
-        <v>2</v>
-      </c>
-      <c r="D4" s="5">
-        <v>2</v>
-      </c>
-      <c r="E4" s="5">
-        <v>2</v>
-      </c>
-      <c r="F4" s="5">
-        <v>2</v>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
       </c>
       <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
+      <c r="H4" s="2">
+        <v>5</v>
+      </c>
+      <c r="I4">
+        <v>5</v>
+      </c>
+      <c r="K4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="5" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -1207,7 +1215,15 @@
       <c r="G29" s="2">
         <v>5</v>
       </c>
-      <c r="H29" s="2"/>
+      <c r="H29" s="2">
+        <v>5</v>
+      </c>
+      <c r="I29" s="6">
+        <v>5</v>
+      </c>
+      <c r="J29" s="6">
+        <v>5</v>
+      </c>
     </row>
     <row r="30" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
@@ -1253,7 +1269,15 @@
       <c r="G31" s="2">
         <v>5</v>
       </c>
-      <c r="H31" s="2"/>
+      <c r="H31" s="2">
+        <v>5</v>
+      </c>
+      <c r="I31" s="6">
+        <v>5</v>
+      </c>
+      <c r="J31" s="6">
+        <v>5</v>
+      </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C32" s="3"/>
@@ -1266,6 +1290,18 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <conditionalFormatting sqref="J4:J31">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D14">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -1277,7 +1313,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D14">
+  <conditionalFormatting sqref="D4">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
AutoCommit_14 июня 2024 г. 9:27:02_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-422_ТерВер.xlsx
+++ b/_2ИСИП-422_ТерВер.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t>2ИСИП-422: Теория вероятностей и математическая статистика (Сибирев И. В.) - II семестр</t>
   </si>
@@ -542,10 +542,10 @@
   <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="L11" sqref="L11"/>
+      <selection pane="bottomRight" activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -773,20 +773,25 @@
       <c r="B11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="5">
-        <v>2</v>
-      </c>
-      <c r="D11" s="5">
-        <v>2</v>
-      </c>
-      <c r="E11" s="5">
-        <v>2</v>
-      </c>
-      <c r="F11" s="5">
-        <v>2</v>
+      <c r="C11" s="6">
+        <v>5</v>
+      </c>
+      <c r="D11" s="6">
+        <v>5</v>
+      </c>
+      <c r="E11" s="6">
+        <v>5</v>
       </c>
       <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
+      <c r="H11" s="2">
+        <v>5</v>
+      </c>
+      <c r="I11">
+        <v>5</v>
+      </c>
+      <c r="K11" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="12" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
@@ -832,7 +837,15 @@
       <c r="G13" s="2">
         <v>5</v>
       </c>
-      <c r="H13" s="2"/>
+      <c r="H13" s="2">
+        <v>5</v>
+      </c>
+      <c r="I13" s="6">
+        <v>5</v>
+      </c>
+      <c r="J13" s="6">
+        <v>5</v>
+      </c>
     </row>
     <row r="14" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
@@ -879,8 +892,18 @@
       <c r="F15" s="5">
         <v>5</v>
       </c>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
+      <c r="G15" s="2">
+        <v>5</v>
+      </c>
+      <c r="H15" s="2">
+        <v>5</v>
+      </c>
+      <c r="I15" s="6">
+        <v>5</v>
+      </c>
+      <c r="J15" s="6">
+        <v>5</v>
+      </c>
     </row>
     <row r="16" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
@@ -928,7 +951,12 @@
       <c r="G17" s="2">
         <v>5</v>
       </c>
-      <c r="H17" s="2"/>
+      <c r="H17" s="2">
+        <v>5</v>
+      </c>
+      <c r="I17" s="6">
+        <v>5</v>
+      </c>
     </row>
     <row r="18" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
@@ -1290,6 +1318,18 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <conditionalFormatting sqref="J4:J31">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D14">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -1301,7 +1341,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D14">
+  <conditionalFormatting sqref="D4">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -1313,7 +1353,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D4">
+  <conditionalFormatting sqref="D11">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
AutoCommit_14 июня 2024 г. 9:53:53_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-422_ТерВер.xlsx
+++ b/_2ИСИП-422_ТерВер.xlsx
@@ -542,10 +542,10 @@
   <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="K15" sqref="K15"/>
+      <selection pane="bottomRight" activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -714,11 +714,21 @@
       <c r="E8" s="5">
         <v>5</v>
       </c>
-      <c r="F8" s="5">
-        <v>2</v>
-      </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
+      <c r="F8" s="2">
+        <v>5</v>
+      </c>
+      <c r="G8" s="2">
+        <v>5</v>
+      </c>
+      <c r="H8" s="2">
+        <v>5</v>
+      </c>
+      <c r="I8" s="7">
+        <v>5</v>
+      </c>
+      <c r="J8" s="7">
+        <v>5</v>
+      </c>
     </row>
     <row r="9" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
@@ -812,8 +822,18 @@
       <c r="F12" s="5">
         <v>5</v>
       </c>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
+      <c r="G12" s="2">
+        <v>5</v>
+      </c>
+      <c r="H12" s="2">
+        <v>5</v>
+      </c>
+      <c r="I12" s="6">
+        <v>5</v>
+      </c>
+      <c r="J12" s="6">
+        <v>5</v>
+      </c>
     </row>
     <row r="13" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
@@ -872,6 +892,12 @@
       <c r="H14" s="2">
         <v>5</v>
       </c>
+      <c r="I14">
+        <v>5</v>
+      </c>
+      <c r="J14">
+        <v>5</v>
+      </c>
     </row>
     <row r="15" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
@@ -1021,8 +1047,18 @@
       <c r="F20" s="5">
         <v>5</v>
       </c>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
+      <c r="G20" s="2">
+        <v>5</v>
+      </c>
+      <c r="H20" s="2">
+        <v>5</v>
+      </c>
+      <c r="I20" s="6">
+        <v>5</v>
+      </c>
+      <c r="J20" s="6">
+        <v>5</v>
+      </c>
     </row>
     <row r="21" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
@@ -1092,7 +1128,15 @@
       <c r="G23" s="2">
         <v>5</v>
       </c>
-      <c r="H23" s="2"/>
+      <c r="H23" s="2">
+        <v>5</v>
+      </c>
+      <c r="I23" s="6">
+        <v>5</v>
+      </c>
+      <c r="J23" s="6">
+        <v>5</v>
+      </c>
     </row>
     <row r="24" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A24" s="1">

</xml_diff>

<commit_message>
AutoCommit_14 июня 2024 г. 9:57:12_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-422_ТерВер.xlsx
+++ b/_2ИСИП-422_ТерВер.xlsx
@@ -542,10 +542,10 @@
   <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I12" sqref="I12"/>
+      <selection pane="bottomRight" activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1316,8 +1316,18 @@
       <c r="F30" s="5">
         <v>5</v>
       </c>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
+      <c r="G30" s="2">
+        <v>5</v>
+      </c>
+      <c r="H30" s="2">
+        <v>5</v>
+      </c>
+      <c r="I30" s="6">
+        <v>5</v>
+      </c>
+      <c r="J30" s="6">
+        <v>5</v>
+      </c>
     </row>
     <row r="31" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A31" s="1">

</xml_diff>

<commit_message>
AutoCommit_14 июня 2024 г. 11:22:33_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-422_ТерВер.xlsx
+++ b/_2ИСИП-422_ТерВер.xlsx
@@ -545,7 +545,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I19" sqref="I19"/>
+      <selection pane="bottomRight" activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1003,8 +1003,18 @@
       <c r="F18" s="5">
         <v>5</v>
       </c>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
+      <c r="G18" s="2">
+        <v>5</v>
+      </c>
+      <c r="H18" s="2">
+        <v>5</v>
+      </c>
+      <c r="I18" s="6">
+        <v>5</v>
+      </c>
+      <c r="J18" s="6">
+        <v>5</v>
+      </c>
     </row>
     <row r="19" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A19" s="1">

</xml_diff>

<commit_message>
AutoCommit_14 июня 2024 г. 13:25:25_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-422_ТерВер.xlsx
+++ b/_2ИСИП-422_ТерВер.xlsx
@@ -551,7 +551,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C25" sqref="C25"/>
+      <selection pane="bottomRight" activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1070,8 +1070,18 @@
       <c r="F19" s="2">
         <v>5</v>
       </c>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
+      <c r="G19" s="2">
+        <v>5</v>
+      </c>
+      <c r="H19" s="2">
+        <v>5</v>
+      </c>
+      <c r="I19" s="8">
+        <v>5</v>
+      </c>
+      <c r="J19" s="9">
+        <v>5</v>
+      </c>
     </row>
     <row r="20" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
@@ -1324,6 +1334,9 @@
         <v>5</v>
       </c>
       <c r="I28" s="8">
+        <v>5</v>
+      </c>
+      <c r="J28">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
AutoCommit_16 июня 2024 г. 8:55:42_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-422_ТерВер.xlsx
+++ b/_2ИСИП-422_ТерВер.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
   <si>
     <t>2ИСИП-422: Теория вероятностей и математическая статистика (Сибирев И. В.) - II семестр</t>
   </si>
@@ -127,13 +127,22 @@
   </si>
   <si>
     <t>Хочу 4</t>
+  </si>
+  <si>
+    <t>ДЗ_6</t>
+  </si>
+  <si>
+    <t>ДЗ_7</t>
+  </si>
+  <si>
+    <t>Сумма</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -143,11 +152,6 @@
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -160,7 +164,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -212,36 +216,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -554,22 +550,22 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J3" sqref="J3"/>
+      <selection pane="bottomRight" activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.1796875" customWidth="1"/>
     <col min="2" max="2" width="41.6328125" customWidth="1"/>
-    <col min="3" max="8" width="5.1796875" customWidth="1"/>
+    <col min="3" max="10" width="5.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="1" t="s">
         <v>28</v>
       </c>
@@ -585,18 +581,21 @@
       <c r="G2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="1">
-        <v>6</v>
-      </c>
-      <c r="I2">
-        <v>7</v>
-      </c>
-      <c r="J2" s="4" t="s">
+      <c r="H2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="K2" s="4"/>
-    </row>
-    <row r="3" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="K2" s="2"/>
+      <c r="L2" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="1">
         <v>1</v>
       </c>
@@ -615,49 +614,56 @@
       <c r="H3" s="1">
         <v>1</v>
       </c>
-      <c r="I3" s="10">
+      <c r="I3" s="3">
         <v>1</v>
       </c>
-      <c r="J3" s="10">
+      <c r="J3" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="13" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4">
-        <v>5</v>
-      </c>
-      <c r="D4">
-        <v>5</v>
-      </c>
-      <c r="E4">
-        <v>5</v>
-      </c>
-      <c r="F4">
-        <v>2</v>
-      </c>
-      <c r="G4" s="2">
-        <v>2</v>
-      </c>
-      <c r="H4" s="2">
-        <v>5</v>
-      </c>
-      <c r="I4">
-        <v>5</v>
-      </c>
-      <c r="J4">
-        <v>2</v>
+      <c r="C4" s="4">
+        <v>5</v>
+      </c>
+      <c r="D4" s="4">
+        <v>5</v>
+      </c>
+      <c r="E4" s="4">
+        <v>5</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0</v>
+      </c>
+      <c r="G4" s="5">
+        <v>0</v>
+      </c>
+      <c r="H4" s="5">
+        <v>5</v>
+      </c>
+      <c r="I4" s="4">
+        <v>5</v>
+      </c>
+      <c r="J4" s="4">
+        <v>0</v>
       </c>
       <c r="K4" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L4">
+        <f>SUM(C4:J4)</f>
+        <v>25</v>
+      </c>
+      <c r="M4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -676,20 +682,27 @@
       <c r="F5" s="5">
         <v>5</v>
       </c>
-      <c r="G5" s="2">
-        <v>2</v>
-      </c>
-      <c r="H5" s="2">
-        <v>2</v>
+      <c r="G5" s="5">
+        <v>0</v>
+      </c>
+      <c r="H5" s="5">
+        <v>0</v>
       </c>
       <c r="I5" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J5" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <f t="shared" ref="L5:L31" si="0">SUM(C5:J5)</f>
+        <v>20</v>
+      </c>
+      <c r="M5" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -705,58 +718,72 @@
       <c r="E6" s="5">
         <v>5</v>
       </c>
-      <c r="F6" s="2">
-        <v>5</v>
-      </c>
-      <c r="G6" s="2">
-        <v>5</v>
-      </c>
-      <c r="H6" s="2">
-        <v>5</v>
-      </c>
-      <c r="I6" s="7">
-        <v>5</v>
-      </c>
-      <c r="J6" s="7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="F6" s="5">
+        <v>5</v>
+      </c>
+      <c r="G6" s="5">
+        <v>5</v>
+      </c>
+      <c r="H6" s="5">
+        <v>5</v>
+      </c>
+      <c r="I6" s="6">
+        <v>5</v>
+      </c>
+      <c r="J6" s="6">
+        <v>5</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="M6" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C7">
-        <v>5</v>
-      </c>
-      <c r="D7">
-        <v>5</v>
-      </c>
-      <c r="E7">
-        <v>5</v>
-      </c>
-      <c r="F7">
-        <v>5</v>
-      </c>
-      <c r="G7" s="2">
-        <v>5</v>
-      </c>
-      <c r="H7" s="2">
-        <v>5</v>
-      </c>
-      <c r="I7">
-        <v>5</v>
-      </c>
-      <c r="J7">
+      <c r="C7" s="4">
+        <v>5</v>
+      </c>
+      <c r="D7" s="4">
+        <v>5</v>
+      </c>
+      <c r="E7" s="4">
+        <v>5</v>
+      </c>
+      <c r="F7" s="4">
+        <v>5</v>
+      </c>
+      <c r="G7" s="5">
+        <v>5</v>
+      </c>
+      <c r="H7" s="5">
+        <v>5</v>
+      </c>
+      <c r="I7" s="4">
+        <v>5</v>
+      </c>
+      <c r="J7" s="4">
         <v>5</v>
       </c>
       <c r="K7" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L7">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="M7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="13" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>5</v>
       </c>
@@ -772,23 +799,30 @@
       <c r="E8" s="5">
         <v>5</v>
       </c>
-      <c r="F8" s="2">
-        <v>5</v>
-      </c>
-      <c r="G8" s="2">
-        <v>5</v>
-      </c>
-      <c r="H8" s="2">
-        <v>5</v>
-      </c>
-      <c r="I8" s="7">
-        <v>5</v>
-      </c>
-      <c r="J8" s="7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="F8" s="5">
+        <v>5</v>
+      </c>
+      <c r="G8" s="5">
+        <v>5</v>
+      </c>
+      <c r="H8" s="5">
+        <v>5</v>
+      </c>
+      <c r="I8" s="6">
+        <v>5</v>
+      </c>
+      <c r="J8" s="6">
+        <v>5</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="M8" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="13" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -807,10 +841,10 @@
       <c r="F9" s="5">
         <v>5</v>
       </c>
-      <c r="G9" s="2">
-        <v>5</v>
-      </c>
-      <c r="H9" s="2">
+      <c r="G9" s="5">
+        <v>5</v>
+      </c>
+      <c r="H9" s="5">
         <v>5</v>
       </c>
       <c r="I9" s="6">
@@ -819,8 +853,15 @@
       <c r="J9" s="6">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L9">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="M9" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="13" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -839,10 +880,10 @@
       <c r="F10" s="5">
         <v>5</v>
       </c>
-      <c r="G10" s="2">
-        <v>5</v>
-      </c>
-      <c r="H10" s="2">
+      <c r="G10" s="5">
+        <v>5</v>
+      </c>
+      <c r="H10" s="5">
         <v>5</v>
       </c>
       <c r="I10" s="6">
@@ -851,8 +892,15 @@
       <c r="J10" s="6">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L10">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="M10" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="13" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -862,32 +910,39 @@
       <c r="C11" s="6">
         <v>5</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="4">
         <v>5</v>
       </c>
       <c r="E11" s="6">
         <v>5</v>
       </c>
-      <c r="F11">
-        <v>2</v>
-      </c>
-      <c r="G11" s="2">
-        <v>2</v>
-      </c>
-      <c r="H11" s="2">
-        <v>5</v>
-      </c>
-      <c r="I11">
-        <v>5</v>
-      </c>
-      <c r="J11">
-        <v>2</v>
+      <c r="F11" s="4">
+        <v>0</v>
+      </c>
+      <c r="G11" s="5">
+        <v>0</v>
+      </c>
+      <c r="H11" s="5">
+        <v>5</v>
+      </c>
+      <c r="I11" s="4">
+        <v>5</v>
+      </c>
+      <c r="J11" s="4">
+        <v>0</v>
       </c>
       <c r="K11" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L11">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="M11" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="13" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -906,10 +961,10 @@
       <c r="F12" s="5">
         <v>5</v>
       </c>
-      <c r="G12" s="2">
-        <v>5</v>
-      </c>
-      <c r="H12" s="2">
+      <c r="G12" s="5">
+        <v>5</v>
+      </c>
+      <c r="H12" s="5">
         <v>5</v>
       </c>
       <c r="I12" s="6">
@@ -918,8 +973,15 @@
       <c r="J12" s="6">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L12">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="M12" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="13" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>10</v>
       </c>
@@ -938,10 +1000,10 @@
       <c r="F13" s="5">
         <v>5</v>
       </c>
-      <c r="G13" s="2">
-        <v>5</v>
-      </c>
-      <c r="H13" s="2">
+      <c r="G13" s="5">
+        <v>5</v>
+      </c>
+      <c r="H13" s="5">
         <v>5</v>
       </c>
       <c r="I13" s="6">
@@ -950,8 +1012,15 @@
       <c r="J13" s="6">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L13">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="M13" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="13" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>11</v>
       </c>
@@ -961,7 +1030,7 @@
       <c r="C14" s="6">
         <v>5</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="4">
         <v>5</v>
       </c>
       <c r="E14" s="6">
@@ -970,20 +1039,27 @@
       <c r="F14" s="6">
         <v>5</v>
       </c>
-      <c r="G14" s="2">
-        <v>5</v>
-      </c>
-      <c r="H14" s="2">
-        <v>5</v>
-      </c>
-      <c r="I14">
-        <v>5</v>
-      </c>
-      <c r="J14">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="G14" s="5">
+        <v>5</v>
+      </c>
+      <c r="H14" s="5">
+        <v>5</v>
+      </c>
+      <c r="I14" s="4">
+        <v>5</v>
+      </c>
+      <c r="J14" s="4">
+        <v>5</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="M14" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="13" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>12</v>
       </c>
@@ -1002,10 +1078,10 @@
       <c r="F15" s="5">
         <v>5</v>
       </c>
-      <c r="G15" s="2">
-        <v>5</v>
-      </c>
-      <c r="H15" s="2">
+      <c r="G15" s="5">
+        <v>5</v>
+      </c>
+      <c r="H15" s="5">
         <v>5</v>
       </c>
       <c r="I15" s="6">
@@ -1014,8 +1090,15 @@
       <c r="J15" s="6">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L15">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="M15" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="13" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>13</v>
       </c>
@@ -1034,16 +1117,23 @@
       <c r="F16" s="5">
         <v>5</v>
       </c>
-      <c r="G16" s="2">
-        <v>5</v>
-      </c>
-      <c r="H16" s="2">
-        <v>5</v>
-      </c>
-      <c r="I16" s="8">
-        <v>5</v>
-      </c>
-      <c r="J16" s="9">
+      <c r="G16" s="5">
+        <v>5</v>
+      </c>
+      <c r="H16" s="5">
+        <v>5</v>
+      </c>
+      <c r="I16" s="7">
+        <v>5</v>
+      </c>
+      <c r="J16" s="8">
+        <v>5</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="M16" s="8">
         <v>5</v>
       </c>
     </row>
@@ -1066,17 +1156,24 @@
       <c r="F17" s="5">
         <v>5</v>
       </c>
-      <c r="G17" s="2">
-        <v>5</v>
-      </c>
-      <c r="H17" s="2">
+      <c r="G17" s="5">
+        <v>5</v>
+      </c>
+      <c r="H17" s="5">
         <v>5</v>
       </c>
       <c r="I17" s="6">
         <v>5</v>
       </c>
-      <c r="J17" s="9">
-        <v>2</v>
+      <c r="J17" s="8">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="M17" s="8">
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="13" x14ac:dyDescent="0.25">
@@ -1098,16 +1195,23 @@
       <c r="F18" s="5">
         <v>5</v>
       </c>
-      <c r="G18" s="2">
-        <v>5</v>
-      </c>
-      <c r="H18" s="2">
+      <c r="G18" s="5">
+        <v>5</v>
+      </c>
+      <c r="H18" s="5">
         <v>5</v>
       </c>
       <c r="I18" s="6">
         <v>5</v>
       </c>
       <c r="J18" s="6">
+        <v>5</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="M18" s="8">
         <v>5</v>
       </c>
     </row>
@@ -1118,28 +1222,35 @@
       <c r="B19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="2">
-        <v>5</v>
-      </c>
-      <c r="D19" s="2">
-        <v>5</v>
-      </c>
-      <c r="E19" s="2">
-        <v>5</v>
-      </c>
-      <c r="F19" s="2">
-        <v>5</v>
-      </c>
-      <c r="G19" s="2">
-        <v>5</v>
-      </c>
-      <c r="H19" s="2">
-        <v>5</v>
-      </c>
-      <c r="I19" s="8">
-        <v>5</v>
-      </c>
-      <c r="J19" s="9">
+      <c r="C19" s="5">
+        <v>5</v>
+      </c>
+      <c r="D19" s="5">
+        <v>5</v>
+      </c>
+      <c r="E19" s="5">
+        <v>5</v>
+      </c>
+      <c r="F19" s="5">
+        <v>5</v>
+      </c>
+      <c r="G19" s="5">
+        <v>5</v>
+      </c>
+      <c r="H19" s="5">
+        <v>5</v>
+      </c>
+      <c r="I19" s="7">
+        <v>5</v>
+      </c>
+      <c r="J19" s="8">
+        <v>5</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="M19" s="8">
         <v>5</v>
       </c>
     </row>
@@ -1162,10 +1273,10 @@
       <c r="F20" s="5">
         <v>5</v>
       </c>
-      <c r="G20" s="2">
-        <v>5</v>
-      </c>
-      <c r="H20" s="2">
+      <c r="G20" s="5">
+        <v>5</v>
+      </c>
+      <c r="H20" s="5">
         <v>5</v>
       </c>
       <c r="I20" s="6">
@@ -1174,45 +1285,59 @@
       <c r="J20" s="6">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+      <c r="L20">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="M20" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>18</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="2">
-        <v>5</v>
-      </c>
-      <c r="D21" s="2">
-        <v>5</v>
-      </c>
-      <c r="E21" s="2">
-        <v>5</v>
-      </c>
-      <c r="F21" s="2">
-        <v>5</v>
-      </c>
-      <c r="G21" s="2">
+      <c r="C21" s="5">
+        <v>5</v>
+      </c>
+      <c r="D21" s="5">
+        <v>5</v>
+      </c>
+      <c r="E21" s="5">
+        <v>5</v>
+      </c>
+      <c r="F21" s="5">
+        <v>5</v>
+      </c>
+      <c r="G21" s="5">
         <v>5</v>
       </c>
       <c r="H21" s="5">
         <v>5</v>
       </c>
-      <c r="I21" s="8">
-        <v>2</v>
-      </c>
-      <c r="J21" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+      <c r="I21" s="7">
+        <v>0</v>
+      </c>
+      <c r="J21" s="8">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="M21" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>19</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="C22" s="5">
         <v>5</v>
@@ -1226,25 +1351,32 @@
       <c r="F22" s="5">
         <v>5</v>
       </c>
-      <c r="G22" s="2">
-        <v>5</v>
-      </c>
-      <c r="H22" s="2">
-        <v>5</v>
-      </c>
-      <c r="I22" s="8">
-        <v>5</v>
-      </c>
-      <c r="J22" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+      <c r="G22" s="5">
+        <v>5</v>
+      </c>
+      <c r="H22" s="5">
+        <v>5</v>
+      </c>
+      <c r="I22" s="6">
+        <v>5</v>
+      </c>
+      <c r="J22" s="6">
+        <v>5</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="M22" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>20</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C23" s="5">
         <v>5</v>
@@ -1258,25 +1390,32 @@
       <c r="F23" s="5">
         <v>5</v>
       </c>
-      <c r="G23" s="2">
-        <v>5</v>
-      </c>
-      <c r="H23" s="2">
+      <c r="G23" s="5">
+        <v>5</v>
+      </c>
+      <c r="H23" s="5">
         <v>5</v>
       </c>
       <c r="I23" s="6">
         <v>5</v>
       </c>
-      <c r="J23" s="6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+      <c r="J23" s="8">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="M23" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>21</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C24" s="5">
         <v>5</v>
@@ -1290,25 +1429,32 @@
       <c r="F24" s="5">
         <v>5</v>
       </c>
-      <c r="G24" s="2">
-        <v>5</v>
-      </c>
-      <c r="H24" s="2">
-        <v>5</v>
-      </c>
-      <c r="I24" s="6">
-        <v>5</v>
-      </c>
-      <c r="J24" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+      <c r="G24" s="5">
+        <v>5</v>
+      </c>
+      <c r="H24" s="5">
+        <v>0</v>
+      </c>
+      <c r="I24" s="7">
+        <v>5</v>
+      </c>
+      <c r="J24" s="8">
+        <v>5</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="M24" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>22</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C25" s="5">
         <v>5</v>
@@ -1322,119 +1468,144 @@
       <c r="F25" s="5">
         <v>5</v>
       </c>
-      <c r="G25" s="2">
-        <v>5</v>
-      </c>
-      <c r="H25" s="2">
-        <v>2</v>
-      </c>
-      <c r="I25" s="8">
-        <v>5</v>
-      </c>
-      <c r="J25" s="9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+      <c r="G25" s="5">
+        <v>5</v>
+      </c>
+      <c r="H25" s="5">
+        <v>5</v>
+      </c>
+      <c r="I25" s="6">
+        <v>5</v>
+      </c>
+      <c r="J25" s="6">
+        <v>5</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="M25" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>23</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C26" s="5">
-        <v>5</v>
-      </c>
-      <c r="D26" s="5">
+        <v>23</v>
+      </c>
+      <c r="C26" s="6">
+        <v>5</v>
+      </c>
+      <c r="D26" s="6">
         <v>5</v>
       </c>
       <c r="E26" s="5">
-        <v>5</v>
-      </c>
-      <c r="F26" s="2">
-        <v>5</v>
-      </c>
-      <c r="G26" s="2">
-        <v>5</v>
-      </c>
-      <c r="H26" s="2">
+        <v>0</v>
+      </c>
+      <c r="F26" s="6">
+        <v>0</v>
+      </c>
+      <c r="G26" s="5">
+        <v>0</v>
+      </c>
+      <c r="H26" s="5">
         <v>5</v>
       </c>
       <c r="I26" s="7">
         <v>5</v>
       </c>
-      <c r="J26" s="7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+      <c r="J26" s="8">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="M26" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>24</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C27" s="6">
-        <v>5</v>
-      </c>
-      <c r="D27" s="6">
-        <v>5</v>
-      </c>
-      <c r="E27" s="6">
-        <v>2</v>
-      </c>
-      <c r="F27" s="6">
-        <v>2</v>
-      </c>
-      <c r="G27" s="2">
-        <v>2</v>
-      </c>
-      <c r="H27" s="2">
-        <v>5</v>
-      </c>
-      <c r="I27" s="8">
-        <v>5</v>
-      </c>
-      <c r="J27" s="9">
-        <v>2</v>
-      </c>
-      <c r="M27">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="C27" s="5">
+        <v>5</v>
+      </c>
+      <c r="D27" s="5">
+        <v>5</v>
+      </c>
+      <c r="E27" s="5">
+        <v>5</v>
+      </c>
+      <c r="F27" s="5">
+        <v>5</v>
+      </c>
+      <c r="G27" s="5">
+        <v>5</v>
+      </c>
+      <c r="H27" s="5">
+        <v>5</v>
+      </c>
+      <c r="I27" s="7">
+        <v>5</v>
+      </c>
+      <c r="J27" s="7">
+        <v>5</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="M27" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>25</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="2">
-        <v>5</v>
-      </c>
-      <c r="D28" s="2">
-        <v>2</v>
-      </c>
-      <c r="E28" s="2">
-        <v>2</v>
-      </c>
-      <c r="F28" s="2">
-        <v>2</v>
-      </c>
-      <c r="G28" s="2">
-        <v>2</v>
-      </c>
-      <c r="H28" s="2">
-        <v>5</v>
-      </c>
-      <c r="I28" s="8">
-        <v>5</v>
-      </c>
-      <c r="J28">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+      <c r="C28" s="5">
+        <v>5</v>
+      </c>
+      <c r="D28" s="5">
+        <v>0</v>
+      </c>
+      <c r="E28" s="5">
+        <v>0</v>
+      </c>
+      <c r="F28" s="5">
+        <v>0</v>
+      </c>
+      <c r="G28" s="5">
+        <v>0</v>
+      </c>
+      <c r="H28" s="5">
+        <v>5</v>
+      </c>
+      <c r="I28" s="7">
+        <v>5</v>
+      </c>
+      <c r="J28" s="4">
+        <v>5</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="M28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>26</v>
       </c>
@@ -1453,10 +1624,10 @@
       <c r="F29" s="5">
         <v>5</v>
       </c>
-      <c r="G29" s="2">
-        <v>5</v>
-      </c>
-      <c r="H29" s="2">
+      <c r="G29" s="5">
+        <v>5</v>
+      </c>
+      <c r="H29" s="5">
         <v>5</v>
       </c>
       <c r="I29" s="6">
@@ -1465,8 +1636,15 @@
       <c r="J29" s="6">
         <v>5</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+      <c r="L29">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="M29" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>27</v>
       </c>
@@ -1485,10 +1663,10 @@
       <c r="F30" s="5">
         <v>5</v>
       </c>
-      <c r="G30" s="2">
-        <v>5</v>
-      </c>
-      <c r="H30" s="2">
+      <c r="G30" s="5">
+        <v>5</v>
+      </c>
+      <c r="H30" s="5">
         <v>5</v>
       </c>
       <c r="I30" s="6">
@@ -1497,8 +1675,15 @@
       <c r="J30" s="6">
         <v>5</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+      <c r="L30">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="M30" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>28</v>
       </c>
@@ -1517,10 +1702,10 @@
       <c r="F31" s="5">
         <v>5</v>
       </c>
-      <c r="G31" s="2">
-        <v>5</v>
-      </c>
-      <c r="H31" s="2">
+      <c r="G31" s="5">
+        <v>5</v>
+      </c>
+      <c r="H31" s="5">
         <v>5</v>
       </c>
       <c r="I31" s="6">
@@ -1529,54 +1714,18 @@
       <c r="J31" s="6">
         <v>5</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
-    </row>
+      <c r="L31">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="M31" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="13" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <conditionalFormatting sqref="J4:J31">
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D14">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D4">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D11">
+  <conditionalFormatting sqref="C4:J31">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -1588,7 +1737,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E27">
+  <conditionalFormatting sqref="L4:L31">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M4:M42">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
AutoCommit_17 июня 2024 г. 13:12:39_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-422_ТерВер.xlsx
+++ b/_2ИСИП-422_ТерВер.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="40">
   <si>
     <t>2ИСИП-422: Теория вероятностей и математическая статистика (Сибирев И. В.) - II семестр</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>Сумма</t>
+  </si>
+  <si>
+    <t>Филиппов Роман</t>
   </si>
 </sst>
 </file>
@@ -544,61 +547,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M32"/>
+  <dimension ref="A1:O33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="K6" sqref="K6"/>
+      <selection pane="bottomRight" activeCell="N32" sqref="N32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.1796875" customWidth="1"/>
-    <col min="2" max="2" width="41.6328125" customWidth="1"/>
-    <col min="3" max="10" width="5.1796875" customWidth="1"/>
+    <col min="2" max="2" width="23.1796875" customWidth="1"/>
+    <col min="3" max="3" width="24.1796875" customWidth="1"/>
+    <col min="4" max="10" width="5.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" t="s">
+    <row r="1" spans="1:15" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="1" t="s">
+    <row r="2" spans="1:15" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="1">
-        <v>1</v>
-      </c>
+    <row r="3" spans="1:15" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D3" s="1">
         <v>1</v>
       </c>
@@ -614,22 +614,25 @@
       <c r="H3" s="1">
         <v>1</v>
       </c>
-      <c r="I3" s="3">
+      <c r="I3" s="1">
         <v>1</v>
       </c>
       <c r="J3" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+      <c r="K3" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>1</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="4">
-        <v>5</v>
+      <c r="C4" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="D4" s="4">
         <v>5</v>
@@ -638,40 +641,43 @@
         <v>5</v>
       </c>
       <c r="F4" s="4">
-        <v>0</v>
-      </c>
-      <c r="G4" s="5">
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="G4" s="4">
+        <v>2</v>
       </c>
       <c r="H4" s="5">
-        <v>5</v>
-      </c>
-      <c r="I4" s="4">
+        <v>2</v>
+      </c>
+      <c r="I4" s="5">
         <v>5</v>
       </c>
       <c r="J4" s="4">
-        <v>0</v>
-      </c>
-      <c r="K4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K4" s="4">
+        <v>2</v>
+      </c>
+      <c r="M4">
+        <f>SUM(D4:K4)</f>
+        <v>31</v>
+      </c>
+      <c r="N4">
+        <v>4</v>
+      </c>
+      <c r="O4" t="s">
         <v>35</v>
       </c>
-      <c r="L4">
-        <f>SUM(C4:J4)</f>
-        <v>25</v>
-      </c>
-      <c r="M4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:15" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>2</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="5">
-        <v>5</v>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="D5" s="5">
         <v>5</v>
@@ -683,34 +689,37 @@
         <v>5</v>
       </c>
       <c r="G5" s="5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H5" s="5">
-        <v>0</v>
-      </c>
-      <c r="I5" s="6">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="I5" s="5">
+        <v>2</v>
       </c>
       <c r="J5" s="6">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <f t="shared" ref="L5:L31" si="0">SUM(C5:J5)</f>
-        <v>20</v>
-      </c>
-      <c r="M5" s="8">
+        <v>2</v>
+      </c>
+      <c r="K5" s="6">
+        <v>2</v>
+      </c>
+      <c r="M5">
+        <f t="shared" ref="M5:M31" si="0">SUM(D5:K5)</f>
+        <v>28</v>
+      </c>
+      <c r="N5" s="8">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>3</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="5">
-        <v>5</v>
+      <c r="C6" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="D6" s="5">
         <v>5</v>
@@ -727,29 +736,32 @@
       <c r="H6" s="5">
         <v>5</v>
       </c>
-      <c r="I6" s="6">
+      <c r="I6" s="5">
         <v>5</v>
       </c>
       <c r="J6" s="6">
         <v>5</v>
       </c>
-      <c r="L6">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="M6" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+      <c r="K6" s="6">
+        <v>5</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="N6" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>4</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="4">
-        <v>5</v>
+      <c r="C7" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="D7" s="4">
         <v>5</v>
@@ -760,37 +772,40 @@
       <c r="F7" s="4">
         <v>5</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="4">
         <v>5</v>
       </c>
       <c r="H7" s="5">
         <v>5</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="5">
         <v>5</v>
       </c>
       <c r="J7" s="4">
         <v>5</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K7" s="4">
+        <v>5</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="N7">
+        <v>5</v>
+      </c>
+      <c r="O7" t="s">
         <v>35</v>
       </c>
-      <c r="L7">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="M7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:15" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>5</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="5">
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="5">
@@ -808,29 +823,32 @@
       <c r="H8" s="5">
         <v>5</v>
       </c>
-      <c r="I8" s="6">
+      <c r="I8" s="5">
         <v>5</v>
       </c>
       <c r="J8" s="6">
         <v>5</v>
       </c>
-      <c r="L8">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="M8" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+      <c r="K8" s="6">
+        <v>5</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="N8" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>6</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="5">
-        <v>5</v>
+      <c r="C9" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="D9" s="5">
         <v>5</v>
@@ -847,29 +865,32 @@
       <c r="H9" s="5">
         <v>5</v>
       </c>
-      <c r="I9" s="6">
+      <c r="I9" s="5">
         <v>5</v>
       </c>
       <c r="J9" s="6">
         <v>5</v>
       </c>
-      <c r="L9">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="M9" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+      <c r="K9" s="6">
+        <v>5</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="N9" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>7</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="5">
-        <v>5</v>
+      <c r="C10" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="D10" s="5">
         <v>5</v>
@@ -886,71 +907,77 @@
       <c r="H10" s="5">
         <v>5</v>
       </c>
-      <c r="I10" s="6">
+      <c r="I10" s="5">
         <v>5</v>
       </c>
       <c r="J10" s="6">
         <v>5</v>
       </c>
-      <c r="L10">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="M10" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+      <c r="K10" s="6">
+        <v>5</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="N10" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>8</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="6">
-        <v>5</v>
-      </c>
-      <c r="D11" s="4">
-        <v>5</v>
-      </c>
-      <c r="E11" s="6">
-        <v>5</v>
-      </c>
-      <c r="F11" s="4">
-        <v>0</v>
-      </c>
-      <c r="G11" s="5">
-        <v>0</v>
+      <c r="C11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="6">
+        <v>5</v>
+      </c>
+      <c r="E11" s="4">
+        <v>5</v>
+      </c>
+      <c r="F11" s="6">
+        <v>5</v>
+      </c>
+      <c r="G11" s="4">
+        <v>2</v>
       </c>
       <c r="H11" s="5">
-        <v>5</v>
-      </c>
-      <c r="I11" s="4">
+        <v>2</v>
+      </c>
+      <c r="I11" s="5">
         <v>5</v>
       </c>
       <c r="J11" s="4">
-        <v>0</v>
-      </c>
-      <c r="K11" t="s">
+        <v>5</v>
+      </c>
+      <c r="K11" s="4">
+        <v>2</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="N11" s="8">
+        <v>4</v>
+      </c>
+      <c r="O11" t="s">
         <v>35</v>
       </c>
-      <c r="L11">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="M11" s="8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:15" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>9</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="5">
-        <v>5</v>
+      <c r="C12" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="D12" s="5">
         <v>5</v>
@@ -967,29 +994,32 @@
       <c r="H12" s="5">
         <v>5</v>
       </c>
-      <c r="I12" s="6">
+      <c r="I12" s="5">
         <v>5</v>
       </c>
       <c r="J12" s="6">
         <v>5</v>
       </c>
-      <c r="L12">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="M12" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+      <c r="K12" s="6">
+        <v>5</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="N12" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>10</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="5">
-        <v>5</v>
+      <c r="C13" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D13" s="5">
         <v>5</v>
@@ -1006,68 +1036,74 @@
       <c r="H13" s="5">
         <v>5</v>
       </c>
-      <c r="I13" s="6">
+      <c r="I13" s="5">
         <v>5</v>
       </c>
       <c r="J13" s="6">
         <v>5</v>
       </c>
-      <c r="L13">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="M13" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+      <c r="K13" s="6">
+        <v>5</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="N13" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>11</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="6">
-        <v>5</v>
-      </c>
-      <c r="D14" s="4">
-        <v>5</v>
-      </c>
-      <c r="E14" s="6">
+      <c r="C14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="6">
+        <v>5</v>
+      </c>
+      <c r="E14" s="4">
         <v>5</v>
       </c>
       <c r="F14" s="6">
         <v>5</v>
       </c>
-      <c r="G14" s="5">
+      <c r="G14" s="6">
         <v>5</v>
       </c>
       <c r="H14" s="5">
         <v>5</v>
       </c>
-      <c r="I14" s="4">
+      <c r="I14" s="5">
         <v>5</v>
       </c>
       <c r="J14" s="4">
         <v>5</v>
       </c>
-      <c r="L14">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="M14" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+      <c r="K14" s="4">
+        <v>5</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="N14" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>12</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="5">
-        <v>5</v>
+      <c r="C15" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="D15" s="5">
         <v>5</v>
@@ -1084,29 +1120,32 @@
       <c r="H15" s="5">
         <v>5</v>
       </c>
-      <c r="I15" s="6">
+      <c r="I15" s="5">
         <v>5</v>
       </c>
       <c r="J15" s="6">
         <v>5</v>
       </c>
-      <c r="L15">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="M15" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+      <c r="K15" s="6">
+        <v>5</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="N15" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>13</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="5">
-        <v>5</v>
+      <c r="C16" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="D16" s="5">
         <v>5</v>
@@ -1123,29 +1162,32 @@
       <c r="H16" s="5">
         <v>5</v>
       </c>
-      <c r="I16" s="7">
-        <v>5</v>
-      </c>
-      <c r="J16" s="8">
-        <v>5</v>
-      </c>
-      <c r="L16">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="M16" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+      <c r="I16" s="5">
+        <v>5</v>
+      </c>
+      <c r="J16" s="7">
+        <v>5</v>
+      </c>
+      <c r="K16" s="8">
+        <v>5</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="N16" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>14</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="5">
-        <v>5</v>
+      <c r="C17" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="D17" s="5">
         <v>5</v>
@@ -1162,29 +1204,32 @@
       <c r="H17" s="5">
         <v>5</v>
       </c>
-      <c r="I17" s="6">
-        <v>5</v>
-      </c>
-      <c r="J17" s="8">
-        <v>0</v>
-      </c>
-      <c r="L17">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="M17" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+      <c r="I17" s="5">
+        <v>5</v>
+      </c>
+      <c r="J17" s="6">
+        <v>5</v>
+      </c>
+      <c r="K17" s="8">
+        <v>2</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="N17" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>15</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="5">
-        <v>5</v>
+      <c r="C18" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="D18" s="5">
         <v>5</v>
@@ -1201,29 +1246,32 @@
       <c r="H18" s="5">
         <v>5</v>
       </c>
-      <c r="I18" s="6">
+      <c r="I18" s="5">
         <v>5</v>
       </c>
       <c r="J18" s="6">
         <v>5</v>
       </c>
-      <c r="L18">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="M18" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+      <c r="K18" s="6">
+        <v>5</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="N18" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>16</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="5">
-        <v>5</v>
+      <c r="C19" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="D19" s="5">
         <v>5</v>
@@ -1240,29 +1288,32 @@
       <c r="H19" s="5">
         <v>5</v>
       </c>
-      <c r="I19" s="7">
-        <v>5</v>
-      </c>
-      <c r="J19" s="8">
-        <v>5</v>
-      </c>
-      <c r="L19">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="M19" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+      <c r="I19" s="5">
+        <v>5</v>
+      </c>
+      <c r="J19" s="7">
+        <v>5</v>
+      </c>
+      <c r="K19" s="8">
+        <v>5</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="N19" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>17</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="5">
-        <v>5</v>
+      <c r="C20" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="D20" s="5">
         <v>5</v>
@@ -1279,29 +1330,32 @@
       <c r="H20" s="5">
         <v>5</v>
       </c>
-      <c r="I20" s="6">
+      <c r="I20" s="5">
         <v>5</v>
       </c>
       <c r="J20" s="6">
         <v>5</v>
       </c>
-      <c r="L20">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="M20" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K20" s="6">
+        <v>5</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="N20" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>18</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="5">
-        <v>5</v>
+      <c r="C21" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="D21" s="5">
         <v>5</v>
@@ -1318,29 +1372,32 @@
       <c r="H21" s="5">
         <v>5</v>
       </c>
-      <c r="I21" s="7">
-        <v>0</v>
-      </c>
-      <c r="J21" s="8">
-        <v>0</v>
-      </c>
-      <c r="L21">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="M21" s="8">
+      <c r="I21" s="5">
+        <v>5</v>
+      </c>
+      <c r="J21" s="7">
+        <v>5</v>
+      </c>
+      <c r="K21" s="8">
+        <v>5</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="N21" s="8">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>19</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="5">
-        <v>5</v>
+      <c r="C22" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D22" s="5">
         <v>5</v>
@@ -1357,29 +1414,32 @@
       <c r="H22" s="5">
         <v>5</v>
       </c>
-      <c r="I22" s="6">
+      <c r="I22" s="5">
         <v>5</v>
       </c>
       <c r="J22" s="6">
         <v>5</v>
       </c>
-      <c r="L22">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="M22" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K22" s="6">
+        <v>5</v>
+      </c>
+      <c r="M22">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="N22" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>20</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="5">
-        <v>5</v>
+      <c r="C23" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="D23" s="5">
         <v>5</v>
@@ -1396,29 +1456,32 @@
       <c r="H23" s="5">
         <v>5</v>
       </c>
-      <c r="I23" s="6">
-        <v>5</v>
-      </c>
-      <c r="J23" s="8">
-        <v>0</v>
-      </c>
-      <c r="L23">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="M23" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I23" s="5">
+        <v>5</v>
+      </c>
+      <c r="J23" s="6">
+        <v>5</v>
+      </c>
+      <c r="K23" s="8">
+        <v>2</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="N23" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>21</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="5">
-        <v>5</v>
+      <c r="C24" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="D24" s="5">
         <v>5</v>
@@ -1433,31 +1496,34 @@
         <v>5</v>
       </c>
       <c r="H24" s="5">
-        <v>0</v>
-      </c>
-      <c r="I24" s="7">
-        <v>5</v>
-      </c>
-      <c r="J24" s="8">
-        <v>5</v>
-      </c>
-      <c r="L24">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="M24" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="I24" s="5">
+        <v>2</v>
+      </c>
+      <c r="J24" s="7">
+        <v>5</v>
+      </c>
+      <c r="K24" s="8">
+        <v>5</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="N24" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>22</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="5">
-        <v>5</v>
+      <c r="C25" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="D25" s="5">
         <v>5</v>
@@ -1474,69 +1540,75 @@
       <c r="H25" s="5">
         <v>5</v>
       </c>
-      <c r="I25" s="6">
+      <c r="I25" s="5">
         <v>5</v>
       </c>
       <c r="J25" s="6">
         <v>5</v>
       </c>
-      <c r="L25">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="M25" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K25" s="6">
+        <v>5</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="N25" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>23</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="6">
-        <v>5</v>
+      <c r="C26" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="D26" s="6">
         <v>5</v>
       </c>
-      <c r="E26" s="5">
-        <v>0</v>
-      </c>
-      <c r="F26" s="6">
-        <v>0</v>
-      </c>
-      <c r="G26" s="5">
-        <v>0</v>
+      <c r="E26" s="6">
+        <v>5</v>
+      </c>
+      <c r="F26" s="5">
+        <v>2</v>
+      </c>
+      <c r="G26" s="6">
+        <v>2</v>
       </c>
       <c r="H26" s="5">
-        <v>5</v>
-      </c>
-      <c r="I26" s="7">
-        <v>5</v>
-      </c>
-      <c r="J26" s="8">
-        <v>0</v>
-      </c>
-      <c r="L26">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="M26" s="8">
+        <v>2</v>
+      </c>
+      <c r="I26" s="5">
+        <v>5</v>
+      </c>
+      <c r="J26" s="7">
+        <v>5</v>
+      </c>
+      <c r="K26" s="8">
+        <v>2</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="N26" s="8">
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>24</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="5">
-        <v>5</v>
-      </c>
       <c r="D27" s="5">
         <v>5</v>
       </c>
@@ -1552,68 +1624,77 @@
       <c r="H27" s="5">
         <v>5</v>
       </c>
-      <c r="I27" s="7">
+      <c r="I27" s="5">
         <v>5</v>
       </c>
       <c r="J27" s="7">
         <v>5</v>
       </c>
-      <c r="L27">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="M27" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K27" s="7">
+        <v>5</v>
+      </c>
+      <c r="M27">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="N27" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>25</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="5">
-        <v>5</v>
+      <c r="C28" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="D28" s="5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E28" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F28" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G28" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H28" s="5">
-        <v>5</v>
-      </c>
-      <c r="I28" s="7">
-        <v>5</v>
-      </c>
-      <c r="J28" s="4">
-        <v>5</v>
-      </c>
-      <c r="L28">
-        <f t="shared" si="0"/>
-        <v>20</v>
+        <v>2</v>
+      </c>
+      <c r="I28" s="5">
+        <v>5</v>
+      </c>
+      <c r="J28" s="7">
+        <v>5</v>
+      </c>
+      <c r="K28" s="4">
+        <v>5</v>
       </c>
       <c r="M28">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="N28">
+        <v>4</v>
+      </c>
+      <c r="O28" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>26</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="5">
-        <v>5</v>
+      <c r="C29" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="D29" s="5">
         <v>5</v>
@@ -1630,29 +1711,32 @@
       <c r="H29" s="5">
         <v>5</v>
       </c>
-      <c r="I29" s="6">
+      <c r="I29" s="5">
         <v>5</v>
       </c>
       <c r="J29" s="6">
         <v>5</v>
       </c>
-      <c r="L29">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="M29" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K29" s="6">
+        <v>5</v>
+      </c>
+      <c r="M29">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="N29" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>27</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="5">
-        <v>5</v>
+      <c r="C30" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="D30" s="5">
         <v>5</v>
@@ -1669,29 +1753,32 @@
       <c r="H30" s="5">
         <v>5</v>
       </c>
-      <c r="I30" s="6">
+      <c r="I30" s="5">
         <v>5</v>
       </c>
       <c r="J30" s="6">
         <v>5</v>
       </c>
-      <c r="L30">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="M30" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K30" s="6">
+        <v>5</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="N30" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>28</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="5">
-        <v>5</v>
+      <c r="C31" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="D31" s="5">
         <v>5</v>
@@ -1708,24 +1795,40 @@
       <c r="H31" s="5">
         <v>5</v>
       </c>
-      <c r="I31" s="6">
+      <c r="I31" s="5">
         <v>5</v>
       </c>
       <c r="J31" s="6">
         <v>5</v>
       </c>
-      <c r="L31">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="M31" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" ht="13" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="K31" s="6">
+        <v>5</v>
+      </c>
+      <c r="M31">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="N31" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <conditionalFormatting sqref="C4:J31">
+  <conditionalFormatting sqref="D4:K31">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L4:L31">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -1737,7 +1840,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L4:L31">
+  <conditionalFormatting sqref="M34:M42 N4:N33">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -1749,7 +1852,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M4:M42">
+  <conditionalFormatting sqref="M4:M31">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>